<commit_message>
Complete the mapping data
</commit_message>
<xml_diff>
--- a/data/final/input/HoaDon2023_Template.xlsx
+++ b/data/final/input/HoaDon2023_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Loclt\Project_out\loclt7\DaElectric\data\final\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE80E30E-3A0B-40E3-BCC2-C3D1040093C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33DF758F-F5FE-4A37-847A-180A0434FA3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{41AB8A55-0524-4A88-A23F-6D1C9F885B49}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
   <si>
     <r>
       <rPr>
@@ -181,10 +181,10 @@
     <t>id=1</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>{{index}}</t>
+    <t>{{unitsInMonth}}</t>
+  </si>
+  <si>
+    <t>{{totalPayment}}</t>
   </si>
 </sst>
 </file>
@@ -383,7 +383,7 @@
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>123113</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -743,10 +743,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72F0112C-AEDF-4C1B-BFFD-89D3F41B2B89}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1100,180 +1100,156 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="17.25" x14ac:dyDescent="0.45">
-      <c r="A3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="1" t="str">
-        <f>B3</f>
-        <v>{{index}}</v>
+    <row r="3" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>14</v>
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="3" t="str">
-        <f>B4</f>
-        <v>{{fullName}}</v>
+        <v>3</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="4" t="e">
-        <f>B5+0</f>
-        <v>#VALUE!</v>
+        <v>4</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="4" t="e">
-        <f>B6+0</f>
-        <v>#VALUE!</v>
+        <v>5</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="4" t="e">
-        <f>B6-B5</f>
-        <v>#VALUE!</v>
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="4" t="e">
-        <f>E6-E5</f>
-        <v>#VALUE!</v>
+        <v>7</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>17</v>
+        <v>8</v>
+      </c>
+      <c r="B8" s="4">
+        <v>20000</v>
       </c>
       <c r="C8" s="4"/>
-      <c r="D8" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="4" t="e">
-        <f>B8+0</f>
-        <v>#VALUE!</v>
+      <c r="D8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="4">
+        <f>B8</f>
+        <v>20000</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4">
-        <v>20000</v>
+        <v>9</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="C9" s="4"/>
-      <c r="D9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="4">
-        <f>B9</f>
-        <v>20000</v>
+      <c r="D9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.4" x14ac:dyDescent="0.45">
-      <c r="A10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="6" t="e">
-        <f>B7*B8+B9</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="6" t="e">
-        <f>B10+0</f>
-        <v>#VALUE!</v>
-      </c>
+    <row r="10" spans="1:5" ht="85.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="14"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="15"/>
     </row>
-    <row r="11" spans="1:5" ht="85.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="15"/>
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="16"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="16" t="str">
+        <f>A11</f>
+        <v>Đak Đoa, ngày      tháng      năm 2024</v>
+      </c>
+      <c r="E11" s="16"/>
     </row>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="16" t="str">
-        <f>A12</f>
-        <v>Đak Đoa, ngày      tháng      năm 2024</v>
-      </c>
-      <c r="E12" s="16"/>
-    </row>
-    <row r="13" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="11" t="s">
+    <row r="12" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="11" t="s">
+      <c r="B12" s="11"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="11"/>
+      <c r="E12" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="D10:E10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="D11:E11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="D12:E12"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.55118110236220474" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="95" orientation="portrait" r:id="rId1"/>

</xml_diff>